<commit_message>
final changes for v1.0
</commit_message>
<xml_diff>
--- a/Inputs/Template for package/Sample_Template_for_Inputs.xlsx
+++ b/Inputs/Template for package/Sample_Template_for_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProxTool_2020\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_CA\ca\Inputs\Template for package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EB4B897-E3EF-4536-A7F3-8FFBC68F26BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772C4651-A592-4FCE-8359-9B1BFBD8F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="660" windowWidth="22455" windowHeight="13830" xr2:uid="{17B2CA14-641E-4D13-8FB6-B3981C43B48E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17B2CA14-641E-4D13-8FB6-B3981C43B48E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,16 +143,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -173,9 +167,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +207,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -319,7 +313,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,16 +466,16 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="3" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -492,114 +486,114 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>-91.132148000000001</v>
+        <v>-91.132099999999994</v>
       </c>
       <c r="C2" s="4">
-        <v>37.636220000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37.636200000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>-95.233680000000007</v>
-      </c>
-      <c r="C3" s="5">
-        <v>40.031182000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-95.233699999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>40.031199999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>-85.417640000000006</v>
-      </c>
-      <c r="C4" s="5">
-        <v>40.156813999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-85.417599999999993</v>
+      </c>
+      <c r="C4" s="4">
+        <v>40.156799999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>-86.299689000000001</v>
-      </c>
-      <c r="C5" s="5">
-        <v>39.755504000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-86.299700000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>39.755499999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3">
-        <v>-82.381994000000006</v>
+        <v>-82.381900000000002</v>
       </c>
       <c r="C6" s="4">
-        <v>27.962440000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27.962399999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3">
-        <v>-85.977526999999995</v>
-      </c>
-      <c r="C7" s="5">
-        <v>31.788311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-85.977500000000006</v>
+      </c>
+      <c r="C7" s="4">
+        <v>31.7883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
-        <v>-117.983931</v>
-      </c>
-      <c r="C8" s="5">
-        <v>34.02514</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>-117.98390000000001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>34.025100000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>-93.118639999999999</v>
-      </c>
-      <c r="C9" s="5">
-        <v>44.834468999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-93.118600000000001</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44.834499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3">
-        <v>-74.359256999999999</v>
-      </c>
-      <c r="C10" s="5">
-        <v>41.460133999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-74.359300000000005</v>
+      </c>
+      <c r="C10" s="4">
+        <v>41.460099999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>-75.766582999999997</v>
-      </c>
-      <c r="C11" s="5">
-        <v>40.470024000000002</v>
+        <v>-75.766599999999997</v>
+      </c>
+      <c r="C11" s="4">
+        <v>40.470100000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>